<commit_message>
Update ref to include line offsets for GPIO
</commit_message>
<xml_diff>
--- a/AML_S905X_CC_REF.xlsx
+++ b/AML_S905X_CC_REF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GKSch\Documents\repos\Lepton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github_Repos\LEPTON\Lepton3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125B4888-0C4A-49B3-9D3C-3C0149C0F85E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC5839B-DB07-4A20-9E7A-1F62BB73FDF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="20376" windowHeight="12360" activeTab="1" xr2:uid="{3EF522ED-8E88-43B6-8797-0B9EE2DC5FD6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{3EF522ED-8E88-43B6-8797-0B9EE2DC5FD6}"/>
   </bookViews>
   <sheets>
     <sheet name="POWER REF 7J1 Header" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
   <si>
     <t>Ethernet Side</t>
   </si>
@@ -177,9 +177,6 @@
     <t>LDTO</t>
   </si>
   <si>
-    <t>spicc-cs1.dts</t>
-  </si>
-  <si>
     <t>AO</t>
   </si>
   <si>
@@ -244,13 +241,19 @@
   </si>
   <si>
     <t>TEST_N</t>
+  </si>
+  <si>
+    <t>spicc-spidev.dts</t>
+  </si>
+  <si>
+    <t>LINE NUM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,6 +266,12 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="9">
@@ -1209,9 +1218,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F34CE76-35A2-4294-88E9-1D1CD38AA65F}">
-  <dimension ref="B2:J26"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1220,19 +1229,24 @@
     <col min="3" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
-        <v>1</v>
-      </c>
+    <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="37" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="37"/>
       <c r="C2" s="37"/>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
-    </row>
-    <row r="4" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="37"/>
+    </row>
+    <row r="4" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>2</v>
+      </c>
       <c r="B4" s="13" t="s">
-        <v>2</v>
+        <v>68</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -1247,10 +1261,14 @@
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="28"/>
       <c r="B5" s="28"/>
       <c r="C5" s="25"/>
       <c r="D5" s="30">
@@ -1262,10 +1280,14 @@
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="3" t="s">
+      <c r="H5" s="28"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -1280,10 +1302,14 @@
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="3" t="s">
+      <c r="H6" s="28"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="B7" s="3">
+        <v>4</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -1298,13 +1324,17 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
       <c r="J7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>98</v>
       </c>
       <c r="C8" s="8">
         <v>1</v>
@@ -1320,11 +1350,15 @@
       <c r="F8" s="4">
         <v>1</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="4">
+        <v>91</v>
+      </c>
+      <c r="H8" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="28"/>
       <c r="B9" s="28"/>
       <c r="C9" s="25"/>
       <c r="D9" s="26">
@@ -1338,13 +1372,19 @@
       <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="4" t="s">
+      <c r="G9" s="4">
+        <v>92</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="3" t="s">
-        <v>66</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8</v>
       </c>
       <c r="C10" s="7">
         <v>0</v>
@@ -1360,13 +1400,19 @@
       <c r="F10" s="3">
         <v>0</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="3">
+        <v>6</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="3" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>12</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9</v>
       </c>
       <c r="C11" s="7">
         <v>0</v>
@@ -1381,10 +1427,14 @@
       </c>
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="3" t="s">
-        <v>67</v>
+      <c r="H11" s="28"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="3">
+        <v>10</v>
       </c>
       <c r="C12" s="7">
         <v>0</v>
@@ -1400,11 +1450,15 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="G12" s="4">
+        <v>93</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="28"/>
       <c r="B13" s="28"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26">
@@ -1418,13 +1472,19 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="4">
+        <v>94</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>13</v>
+      </c>
+      <c r="B14" s="4">
+        <v>87</v>
       </c>
       <c r="C14" s="8">
         <v>1</v>
@@ -1439,10 +1499,14 @@
       </c>
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="H14" s="28"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>14</v>
+      </c>
+      <c r="B15" s="4">
+        <v>88</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
@@ -1458,13 +1522,19 @@
       <c r="F15" s="4">
         <v>1</v>
       </c>
-      <c r="G15" s="4" t="s">
+      <c r="G15" s="4">
+        <v>79</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>15</v>
+      </c>
+      <c r="B16" s="4">
+        <v>90</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
@@ -1480,11 +1550,15 @@
       <c r="F16" s="4">
         <v>1</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="4">
+        <v>89</v>
+      </c>
+      <c r="H16" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="28"/>
       <c r="B17" s="28"/>
       <c r="C17" s="25"/>
       <c r="D17" s="26">
@@ -1498,13 +1572,19 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="4">
+        <v>80</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="B18" s="4">
+        <v>75</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
@@ -1520,13 +1600,19 @@
       <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="G18" s="4">
+        <v>76</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
         <v>17</v>
+      </c>
+      <c r="B19" s="4">
+        <v>96</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
@@ -1541,10 +1627,14 @@
       </c>
       <c r="F19" s="28"/>
       <c r="G19" s="28"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="H19" s="28"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>18</v>
+      </c>
+      <c r="B20" s="4">
+        <v>97</v>
       </c>
       <c r="C20" s="8">
         <v>1</v>
@@ -1560,13 +1650,19 @@
       <c r="F20" s="4">
         <v>1</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="4">
+        <v>95</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="B21" s="4">
+        <v>85</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
@@ -1581,10 +1677,14 @@
       </c>
       <c r="F21" s="28"/>
       <c r="G21" s="28"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="H21" s="28"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
         <v>20</v>
+      </c>
+      <c r="B22" s="4">
+        <v>86</v>
       </c>
       <c r="C22" s="8">
         <v>1</v>
@@ -1600,13 +1700,19 @@
       <c r="F22" s="4">
         <v>1</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="4">
+        <v>81</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>21</v>
+      </c>
+      <c r="B23" s="4">
+        <v>84</v>
       </c>
       <c r="C23" s="8">
         <v>1</v>
@@ -1622,11 +1728,15 @@
       <c r="F23" s="4">
         <v>1</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="4">
+        <v>82</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="28"/>
       <c r="B24" s="28"/>
       <c r="C24" s="25"/>
       <c r="D24" s="32">
@@ -1640,26 +1750,32 @@
       <c r="F24" s="4">
         <v>1</v>
       </c>
-      <c r="G24" s="4" t="s">
+      <c r="G24" s="4">
+        <v>83</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="13.8" thickTop="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="37" t="s">
+    <row r="25" spans="1:8" ht="13.8" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="37" t="s">
         <v>0</v>
       </c>
+      <c r="B26" s="37"/>
       <c r="C26" s="37"/>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
       <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B26:G26"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A26:H26"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1669,7 +1785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D23D83D7-7A48-48FF-BC6E-37BC984358A3}">
   <dimension ref="B2:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1696,7 +1812,7 @@
     </row>
     <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -1711,7 +1827,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I4" s="38" t="s">
         <v>44</v>
@@ -1732,10 +1848,10 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="I5" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
@@ -1756,10 +1872,10 @@
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="I6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
@@ -2062,7 +2178,7 @@
     <col min="1" max="1" width="10" style="1"/>
     <col min="2" max="2" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="10" style="1"/>
-    <col min="9" max="9" width="11.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
@@ -2078,7 +2194,7 @@
     </row>
     <row r="4" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -2093,7 +2209,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>44</v>
@@ -2112,7 +2228,7 @@
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="I5" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
@@ -2129,7 +2245,7 @@
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="I6" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
@@ -2426,7 +2542,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823D38CA-B1B7-4F85-88F2-26313FEA241E}">
-  <dimension ref="B2:J26"/>
+  <dimension ref="B2:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2437,7 +2553,7 @@
     <col min="3" max="16384" width="10" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="37" t="s">
         <v>1</v>
       </c>
@@ -2447,9 +2563,9 @@
       <c r="F2" s="37"/>
       <c r="G2" s="37"/>
     </row>
-    <row r="4" spans="2:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:7" ht="13.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="13" t="s">
         <v>3</v>
@@ -2464,14 +2580,10 @@
         <v>3</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I4" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="2:10" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="13.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B5" s="28"/>
       <c r="C5" s="25"/>
       <c r="D5" s="30">
@@ -2483,12 +2595,10 @@
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="7">
         <v>0</v>
@@ -2503,12 +2613,10 @@
       </c>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7">
         <v>0</v>
@@ -2523,11 +2631,8 @@
       </c>
       <c r="F7" s="28"/>
       <c r="G7" s="28"/>
-      <c r="J7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="28"/>
       <c r="C8" s="25"/>
       <c r="D8" s="26">
@@ -2542,10 +2647,10 @@
         <v>1</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="28"/>
       <c r="C9" s="25"/>
       <c r="D9" s="26">
@@ -2560,10 +2665,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="28"/>
       <c r="C10" s="25"/>
       <c r="D10" s="26">
@@ -2577,7 +2682,7 @@
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="28"/>
       <c r="C11" s="25"/>
       <c r="D11" s="26">
@@ -2591,7 +2696,7 @@
       <c r="F11" s="28"/>
       <c r="G11" s="28"/>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="28"/>
       <c r="C12" s="25"/>
       <c r="D12" s="26">
@@ -2606,10 +2711,10 @@
         <v>1</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="28"/>
       <c r="C13" s="25"/>
       <c r="D13" s="26">
@@ -2624,12 +2729,12 @@
         <v>1</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="22">
         <v>1</v>
@@ -2645,30 +2750,30 @@
       <c r="F14" s="28"/>
       <c r="G14" s="28"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1</v>
+      </c>
+      <c r="D15" s="23">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="E15" s="27">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="F15" s="28">
+        <v>1</v>
+      </c>
+      <c r="G15" s="28"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="22">
-        <v>1</v>
-      </c>
-      <c r="D15" s="23">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="E15" s="27">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="F15" s="28">
-        <v>1</v>
-      </c>
-      <c r="G15" s="28"/>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="14" t="s">
-        <v>54</v>
-      </c>
       <c r="C16" s="22">
         <v>1</v>
       </c>
@@ -2684,7 +2789,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
@@ -2705,7 +2810,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B18" s="33" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="34">
         <v>1</v>
@@ -2722,7 +2827,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
@@ -2829,10 +2934,9 @@
       <c r="G26" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B26:G26"/>
-    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>